<commit_message>
send mails to student
</commit_message>
<xml_diff>
--- a/Unified_Student_System.xlsx
+++ b/Unified_Student_System.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\~VS Code Saves\ELMS Torneros\python create excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\~VS Code Saves\ELMS Torneros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC904B7-93CD-4438-A86F-87E4CE8757AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA3C400-12B1-4F6A-950E-7296F57CAA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2104" uniqueCount="291">
   <si>
     <t>student_id</t>
   </si>
@@ -898,13 +898,22 @@
   </si>
   <si>
     <t>year_level</t>
+  </si>
+  <si>
+    <t>100050</t>
+  </si>
+  <si>
+    <t>Adrian Angeles</t>
+  </si>
+  <si>
+    <t>adrianangeles2212@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -914,6 +923,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -999,10 +1016,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1014,11 +1032,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1044,27 +1086,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC7E6A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1217,8 +1238,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="GradesTable" displayName="GradesTable" ref="A1:K451" dataDxfId="18">
-  <autoFilter ref="A1:K451" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="GradesTable" displayName="GradesTable" ref="A1:K460" dataDxfId="18">
+  <autoFilter ref="A1:K460" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K451">
     <sortCondition ref="A1:A451"/>
   </sortState>
@@ -1528,8 +1549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2448,7 +2469,7 @@
         <v>174</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" ref="E34:E65" ca="1" si="1">IF(D34="","",DATEDIF(D34,TODAY(),"Y"))</f>
+        <f t="shared" ref="E34:E51" ca="1" si="1">IF(D34="","",DATEDIF(D34,TODAY(),"Y"))</f>
         <v>21</v>
       </c>
       <c r="F34" t="s">
@@ -2921,7 +2942,31 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B52" s="5"/>
+      <c r="A52" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="C52" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="11">
+        <v>38055</v>
+      </c>
+      <c r="E52" s="1">
+        <f ca="1">IF(D52="","",DATEDIF(D52,TODAY(),"Y"))</f>
+        <v>21</v>
+      </c>
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52">
+        <v>9762607481</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>290</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2930,10 +2975,13 @@
       <formula1>"Male,Female"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H52" r:id="rId1" xr:uid="{AD83549E-62D1-4F20-8FE4-131E6CC41E4C}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2942,8 +2990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O927"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A427" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H451" sqref="H451"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3001,7 +3049,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
-        <f>IFERROR(Students!B13, "Student Not Found")</f>
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
         <v>Alex Aquino</v>
       </c>
       <c r="B2" t="s">
@@ -3039,8 +3087,9 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>68</v>
+      <c r="A3" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B3" t="s">
         <v>269</v>
@@ -3077,8 +3126,9 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>68</v>
+      <c r="A4" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B4" t="s">
         <v>272</v>
@@ -3115,8 +3165,9 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>68</v>
+      <c r="A5" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B5" t="s">
         <v>280</v>
@@ -3153,8 +3204,9 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>68</v>
+      <c r="A6" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B6" t="s">
         <v>282</v>
@@ -3191,8 +3243,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>68</v>
+      <c r="A7" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B7" t="s">
         <v>278</v>
@@ -3229,8 +3282,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>68</v>
+      <c r="A8" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B8" t="s">
         <v>277</v>
@@ -3267,8 +3321,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>68</v>
+      <c r="A9" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B9" t="s">
         <v>273</v>
@@ -3303,8 +3358,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>68</v>
+      <c r="A10" s="5" t="str">
+        <f>IFERROR(Students!B$13, "Student Not Found")</f>
+        <v>Alex Aquino</v>
       </c>
       <c r="B10" t="s">
         <v>275</v>
@@ -13171,7 +13227,7 @@
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="5" t="str">
-        <f>IFERROR(Students!B18, "Student Not Found")</f>
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
         <v>Bea Santos</v>
       </c>
       <c r="B272" s="7" t="s">
@@ -13209,8 +13265,9 @@
       </c>
     </row>
     <row r="273" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A273" s="5" t="s">
-        <v>93</v>
+      <c r="A273" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B273" s="7" t="s">
         <v>269</v>
@@ -13247,8 +13304,9 @@
       </c>
     </row>
     <row r="274" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A274" s="5" t="s">
-        <v>93</v>
+      <c r="A274" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B274" s="7" t="s">
         <v>272</v>
@@ -13285,8 +13343,9 @@
       </c>
     </row>
     <row r="275" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A275" s="5" t="s">
-        <v>93</v>
+      <c r="A275" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B275" s="7" t="s">
         <v>280</v>
@@ -13323,8 +13382,9 @@
       </c>
     </row>
     <row r="276" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A276" s="5" t="s">
-        <v>93</v>
+      <c r="A276" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B276" s="7" t="s">
         <v>282</v>
@@ -13361,8 +13421,9 @@
       </c>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A277" s="5" t="s">
-        <v>93</v>
+      <c r="A277" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B277" s="7" t="s">
         <v>278</v>
@@ -13399,8 +13460,9 @@
       </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A278" s="5" t="s">
-        <v>93</v>
+      <c r="A278" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B278" s="7" t="s">
         <v>277</v>
@@ -13437,8 +13499,9 @@
       </c>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A279" s="5" t="s">
-        <v>93</v>
+      <c r="A279" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B279" s="7" t="s">
         <v>273</v>
@@ -13473,8 +13536,9 @@
       </c>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A280" s="5" t="s">
-        <v>93</v>
+      <c r="A280" s="5" t="str">
+        <f>IFERROR(Students!B$18, "Student Not Found")</f>
+        <v>Bea Santos</v>
       </c>
       <c r="B280" s="7" t="s">
         <v>275</v>
@@ -13510,7 +13574,7 @@
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="5" t="str">
-        <f>IFERROR(Students!B26, "Student Not Found")</f>
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
         <v>Bea Torres</v>
       </c>
       <c r="B281" s="7" t="s">
@@ -13548,8 +13612,9 @@
       </c>
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A282" s="5" t="s">
-        <v>133</v>
+      <c r="A282" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B282" s="7" t="s">
         <v>269</v>
@@ -13586,8 +13651,9 @@
       </c>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A283" s="5" t="s">
-        <v>133</v>
+      <c r="A283" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B283" s="7" t="s">
         <v>272</v>
@@ -13624,8 +13690,9 @@
       </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A284" s="5" t="s">
-        <v>133</v>
+      <c r="A284" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B284" s="7" t="s">
         <v>280</v>
@@ -13662,8 +13729,9 @@
       </c>
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A285" s="5" t="s">
-        <v>133</v>
+      <c r="A285" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B285" s="7" t="s">
         <v>282</v>
@@ -13700,8 +13768,9 @@
       </c>
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A286" s="5" t="s">
-        <v>133</v>
+      <c r="A286" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B286" s="7" t="s">
         <v>278</v>
@@ -13738,8 +13807,9 @@
       </c>
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A287" s="5" t="s">
-        <v>133</v>
+      <c r="A287" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B287" s="7" t="s">
         <v>277</v>
@@ -13776,8 +13846,9 @@
       </c>
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A288" s="5" t="s">
-        <v>133</v>
+      <c r="A288" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B288" s="7" t="s">
         <v>273</v>
@@ -13812,8 +13883,9 @@
       </c>
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A289" s="5" t="s">
-        <v>133</v>
+      <c r="A289" s="5" t="str">
+        <f>IFERROR(Students!B$26, "Student Not Found")</f>
+        <v>Bea Torres</v>
       </c>
       <c r="B289" s="7" t="s">
         <v>275</v>
@@ -13849,7 +13921,7 @@
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="5" t="str">
-        <f>IFERROR(Students!B45, "Student Not Found")</f>
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
         <v>Carlo Aquino</v>
       </c>
       <c r="B290" s="7" t="s">
@@ -13887,8 +13959,9 @@
       </c>
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A291" s="5" t="s">
-        <v>228</v>
+      <c r="A291" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B291" s="7" t="s">
         <v>269</v>
@@ -13925,8 +13998,9 @@
       </c>
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A292" s="5" t="s">
-        <v>228</v>
+      <c r="A292" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B292" s="7" t="s">
         <v>272</v>
@@ -13963,8 +14037,9 @@
       </c>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A293" s="5" t="s">
-        <v>228</v>
+      <c r="A293" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B293" s="7" t="s">
         <v>280</v>
@@ -14001,8 +14076,9 @@
       </c>
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A294" s="5" t="s">
-        <v>228</v>
+      <c r="A294" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B294" s="7" t="s">
         <v>282</v>
@@ -14039,8 +14115,9 @@
       </c>
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A295" s="5" t="s">
-        <v>228</v>
+      <c r="A295" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B295" s="7" t="s">
         <v>278</v>
@@ -14077,8 +14154,9 @@
       </c>
     </row>
     <row r="296" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A296" s="5" t="s">
-        <v>228</v>
+      <c r="A296" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B296" s="7" t="s">
         <v>277</v>
@@ -14113,8 +14191,9 @@
       </c>
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A297" s="5" t="s">
-        <v>228</v>
+      <c r="A297" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B297" s="7" t="s">
         <v>273</v>
@@ -14149,8 +14228,9 @@
       </c>
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A298" s="5" t="s">
-        <v>228</v>
+      <c r="A298" s="5" t="str">
+        <f>IFERROR(Students!B$45, "Student Not Found")</f>
+        <v>Carlo Aquino</v>
       </c>
       <c r="B298" s="7" t="s">
         <v>275</v>
@@ -14186,7 +14266,7 @@
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="5" t="str">
-        <f>IFERROR(Students!B47, "Student Not Found")</f>
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
         <v>Carlo Castro</v>
       </c>
       <c r="B299" s="7" t="s">
@@ -14224,8 +14304,9 @@
       </c>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A300" s="5" t="s">
-        <v>238</v>
+      <c r="A300" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B300" s="7" t="s">
         <v>269</v>
@@ -14262,8 +14343,9 @@
       </c>
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A301" s="5" t="s">
-        <v>238</v>
+      <c r="A301" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B301" s="7" t="s">
         <v>272</v>
@@ -14300,8 +14382,9 @@
       </c>
     </row>
     <row r="302" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A302" s="5" t="s">
-        <v>238</v>
+      <c r="A302" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B302" s="7" t="s">
         <v>280</v>
@@ -14338,8 +14421,9 @@
       </c>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A303" s="5" t="s">
-        <v>238</v>
+      <c r="A303" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B303" s="7" t="s">
         <v>282</v>
@@ -14376,8 +14460,9 @@
       </c>
     </row>
     <row r="304" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A304" s="5" t="s">
-        <v>238</v>
+      <c r="A304" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B304" s="7" t="s">
         <v>278</v>
@@ -14414,8 +14499,9 @@
       </c>
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A305" s="5" t="s">
-        <v>238</v>
+      <c r="A305" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B305" s="7" t="s">
         <v>277</v>
@@ -14450,8 +14536,9 @@
       </c>
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A306" s="5" t="s">
-        <v>238</v>
+      <c r="A306" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B306" s="7" t="s">
         <v>273</v>
@@ -14486,8 +14573,9 @@
       </c>
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A307" s="5" t="s">
-        <v>238</v>
+      <c r="A307" s="5" t="str">
+        <f>IFERROR(Students!B$47, "Student Not Found")</f>
+        <v>Carlo Castro</v>
       </c>
       <c r="B307" s="7" t="s">
         <v>275</v>
@@ -14523,7 +14611,7 @@
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="5" t="str">
-        <f>IFERROR(Students!B37, "Student Not Found")</f>
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
         <v>Carlo Cruz</v>
       </c>
       <c r="B308" s="7" t="s">
@@ -14561,8 +14649,9 @@
       </c>
     </row>
     <row r="309" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A309" s="5" t="s">
-        <v>188</v>
+      <c r="A309" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B309" s="7" t="s">
         <v>269</v>
@@ -14599,8 +14688,9 @@
       </c>
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A310" s="5" t="s">
-        <v>188</v>
+      <c r="A310" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B310" s="7" t="s">
         <v>272</v>
@@ -14637,8 +14727,9 @@
       </c>
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A311" s="5" t="s">
-        <v>188</v>
+      <c r="A311" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B311" s="7" t="s">
         <v>280</v>
@@ -14675,8 +14766,9 @@
       </c>
     </row>
     <row r="312" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A312" s="5" t="s">
-        <v>188</v>
+      <c r="A312" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B312" s="7" t="s">
         <v>282</v>
@@ -14713,8 +14805,9 @@
       </c>
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A313" s="5" t="s">
-        <v>188</v>
+      <c r="A313" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B313" s="7" t="s">
         <v>278</v>
@@ -14751,8 +14844,9 @@
       </c>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A314" s="5" t="s">
-        <v>188</v>
+      <c r="A314" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B314" s="7" t="s">
         <v>277</v>
@@ -14789,8 +14883,9 @@
       </c>
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A315" s="5" t="s">
-        <v>188</v>
+      <c r="A315" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B315" s="7" t="s">
         <v>273</v>
@@ -14825,8 +14920,9 @@
       </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A316" s="5" t="s">
-        <v>188</v>
+      <c r="A316" s="5" t="str">
+        <f>IFERROR(Students!B$37, "Student Not Found")</f>
+        <v>Carlo Cruz</v>
       </c>
       <c r="B316" s="7" t="s">
         <v>275</v>
@@ -14862,7 +14958,7 @@
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="5" t="str">
-        <f>IFERROR(Students!B48, "Student Not Found")</f>
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
         <v>Carlo Delos Reyes</v>
       </c>
       <c r="B317" s="7" t="s">
@@ -14900,8 +14996,9 @@
       </c>
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A318" s="5" t="s">
-        <v>243</v>
+      <c r="A318" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B318" s="7" t="s">
         <v>269</v>
@@ -14938,8 +15035,9 @@
       </c>
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A319" s="5" t="s">
-        <v>243</v>
+      <c r="A319" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B319" s="7" t="s">
         <v>272</v>
@@ -14976,8 +15074,9 @@
       </c>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A320" s="5" t="s">
-        <v>243</v>
+      <c r="A320" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B320" s="7" t="s">
         <v>280</v>
@@ -15014,8 +15113,9 @@
       </c>
     </row>
     <row r="321" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A321" s="5" t="s">
-        <v>243</v>
+      <c r="A321" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B321" s="7" t="s">
         <v>282</v>
@@ -15052,8 +15152,9 @@
       </c>
     </row>
     <row r="322" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A322" s="5" t="s">
-        <v>243</v>
+      <c r="A322" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B322" s="7" t="s">
         <v>278</v>
@@ -15090,8 +15191,9 @@
       </c>
     </row>
     <row r="323" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A323" s="5" t="s">
-        <v>243</v>
+      <c r="A323" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B323" s="7" t="s">
         <v>277</v>
@@ -15126,8 +15228,9 @@
       </c>
     </row>
     <row r="324" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A324" s="5" t="s">
-        <v>243</v>
+      <c r="A324" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B324" s="7" t="s">
         <v>273</v>
@@ -15162,8 +15265,9 @@
       </c>
     </row>
     <row r="325" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A325" s="5" t="s">
-        <v>243</v>
+      <c r="A325" s="5" t="str">
+        <f>IFERROR(Students!B$48, "Student Not Found")</f>
+        <v>Carlo Delos Reyes</v>
       </c>
       <c r="B325" s="7" t="s">
         <v>275</v>
@@ -15199,7 +15303,7 @@
     </row>
     <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="5" t="str">
-        <f>IFERROR(Students!B39, "Student Not Found")</f>
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
         <v>Carlo Flores</v>
       </c>
       <c r="B326" s="7" t="s">
@@ -15237,8 +15341,9 @@
       </c>
     </row>
     <row r="327" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A327" s="5" t="s">
-        <v>198</v>
+      <c r="A327" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B327" s="7" t="s">
         <v>269</v>
@@ -15275,8 +15380,9 @@
       </c>
     </row>
     <row r="328" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A328" s="5" t="s">
-        <v>198</v>
+      <c r="A328" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B328" s="7" t="s">
         <v>272</v>
@@ -15313,8 +15419,9 @@
       </c>
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A329" s="5" t="s">
-        <v>198</v>
+      <c r="A329" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B329" s="7" t="s">
         <v>280</v>
@@ -15351,8 +15458,9 @@
       </c>
     </row>
     <row r="330" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A330" s="5" t="s">
-        <v>198</v>
+      <c r="A330" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B330" s="7" t="s">
         <v>282</v>
@@ -15389,8 +15497,9 @@
       </c>
     </row>
     <row r="331" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A331" s="5" t="s">
-        <v>198</v>
+      <c r="A331" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B331" s="7" t="s">
         <v>278</v>
@@ -15427,8 +15536,9 @@
       </c>
     </row>
     <row r="332" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A332" s="5" t="s">
-        <v>198</v>
+      <c r="A332" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B332" s="7" t="s">
         <v>277</v>
@@ -15465,8 +15575,9 @@
       </c>
     </row>
     <row r="333" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A333" s="5" t="s">
-        <v>198</v>
+      <c r="A333" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B333" s="7" t="s">
         <v>273</v>
@@ -15501,8 +15612,9 @@
       </c>
     </row>
     <row r="334" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A334" s="5" t="s">
-        <v>198</v>
+      <c r="A334" s="5" t="str">
+        <f>IFERROR(Students!B$39, "Student Not Found")</f>
+        <v>Carlo Flores</v>
       </c>
       <c r="B334" s="7" t="s">
         <v>275</v>
@@ -15538,7 +15650,7 @@
     </row>
     <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="5" t="str">
-        <f>IFERROR(Students!B35, "Student Not Found")</f>
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
         <v>Carlo Garcia</v>
       </c>
       <c r="B335" s="7" t="s">
@@ -15576,8 +15688,9 @@
       </c>
     </row>
     <row r="336" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A336" s="5" t="s">
-        <v>178</v>
+      <c r="A336" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B336" s="7" t="s">
         <v>269</v>
@@ -15614,8 +15727,9 @@
       </c>
     </row>
     <row r="337" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A337" s="5" t="s">
-        <v>178</v>
+      <c r="A337" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B337" s="7" t="s">
         <v>272</v>
@@ -15652,8 +15766,9 @@
       </c>
     </row>
     <row r="338" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A338" s="5" t="s">
-        <v>178</v>
+      <c r="A338" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B338" s="7" t="s">
         <v>280</v>
@@ -15690,8 +15805,9 @@
       </c>
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A339" s="5" t="s">
-        <v>178</v>
+      <c r="A339" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B339" s="7" t="s">
         <v>282</v>
@@ -15728,8 +15844,9 @@
       </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A340" s="5" t="s">
-        <v>178</v>
+      <c r="A340" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B340" s="7" t="s">
         <v>278</v>
@@ -15766,8 +15883,9 @@
       </c>
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A341" s="5" t="s">
-        <v>178</v>
+      <c r="A341" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B341" s="7" t="s">
         <v>277</v>
@@ -15804,8 +15922,9 @@
       </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A342" s="5" t="s">
-        <v>178</v>
+      <c r="A342" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B342" s="7" t="s">
         <v>273</v>
@@ -15840,8 +15959,9 @@
       </c>
     </row>
     <row r="343" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A343" s="5" t="s">
-        <v>178</v>
+      <c r="A343" s="5" t="str">
+        <f>IFERROR(Students!B$35, "Student Not Found")</f>
+        <v>Carlo Garcia</v>
       </c>
       <c r="B343" s="7" t="s">
         <v>275</v>
@@ -15877,7 +15997,7 @@
     </row>
     <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="5" t="str">
-        <f>IFERROR(Students!B41, "Student Not Found")</f>
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
         <v>Carlo Gonzales</v>
       </c>
       <c r="B344" s="7" t="s">
@@ -15915,8 +16035,9 @@
       </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A345" s="5" t="s">
-        <v>208</v>
+      <c r="A345" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B345" s="7" t="s">
         <v>269</v>
@@ -15953,8 +16074,9 @@
       </c>
     </row>
     <row r="346" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A346" s="5" t="s">
-        <v>208</v>
+      <c r="A346" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B346" s="7" t="s">
         <v>272</v>
@@ -15991,8 +16113,9 @@
       </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A347" s="5" t="s">
-        <v>208</v>
+      <c r="A347" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B347" s="7" t="s">
         <v>280</v>
@@ -16029,8 +16152,9 @@
       </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A348" s="5" t="s">
-        <v>208</v>
+      <c r="A348" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B348" s="7" t="s">
         <v>282</v>
@@ -16067,8 +16191,9 @@
       </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A349" s="5" t="s">
-        <v>208</v>
+      <c r="A349" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B349" s="7" t="s">
         <v>278</v>
@@ -16105,8 +16230,9 @@
       </c>
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A350" s="5" t="s">
-        <v>208</v>
+      <c r="A350" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B350" s="7" t="s">
         <v>277</v>
@@ -16141,8 +16267,9 @@
       </c>
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A351" s="5" t="s">
-        <v>208</v>
+      <c r="A351" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B351" s="7" t="s">
         <v>273</v>
@@ -16177,8 +16304,9 @@
       </c>
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A352" s="5" t="s">
-        <v>208</v>
+      <c r="A352" s="5" t="str">
+        <f>IFERROR(Students!B$41, "Student Not Found")</f>
+        <v>Carlo Gonzales</v>
       </c>
       <c r="B352" s="7" t="s">
         <v>275</v>
@@ -16214,7 +16342,7 @@
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="5" t="str">
-        <f>IFERROR(Students!B38, "Student Not Found")</f>
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
         <v>Carlo Lopez</v>
       </c>
       <c r="B353" s="7" t="s">
@@ -16252,8 +16380,9 @@
       </c>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A354" s="5" t="s">
-        <v>193</v>
+      <c r="A354" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B354" s="7" t="s">
         <v>269</v>
@@ -16290,8 +16419,9 @@
       </c>
     </row>
     <row r="355" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A355" s="5" t="s">
-        <v>193</v>
+      <c r="A355" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B355" s="7" t="s">
         <v>272</v>
@@ -16328,8 +16458,9 @@
       </c>
     </row>
     <row r="356" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A356" s="5" t="s">
-        <v>193</v>
+      <c r="A356" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B356" s="7" t="s">
         <v>280</v>
@@ -16366,8 +16497,9 @@
       </c>
     </row>
     <row r="357" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A357" s="5" t="s">
-        <v>193</v>
+      <c r="A357" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B357" s="7" t="s">
         <v>282</v>
@@ -16404,8 +16536,9 @@
       </c>
     </row>
     <row r="358" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A358" s="5" t="s">
-        <v>193</v>
+      <c r="A358" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B358" s="7" t="s">
         <v>278</v>
@@ -16442,8 +16575,9 @@
       </c>
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A359" s="5" t="s">
-        <v>193</v>
+      <c r="A359" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B359" s="7" t="s">
         <v>277</v>
@@ -16480,8 +16614,9 @@
       </c>
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A360" s="5" t="s">
-        <v>193</v>
+      <c r="A360" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B360" s="7" t="s">
         <v>273</v>
@@ -16516,8 +16651,9 @@
       </c>
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A361" s="5" t="s">
-        <v>193</v>
+      <c r="A361" s="5" t="str">
+        <f>IFERROR(Students!B$38, "Student Not Found")</f>
+        <v>Carlo Lopez</v>
       </c>
       <c r="B361" s="7" t="s">
         <v>275</v>
@@ -16591,8 +16727,9 @@
       </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A363" s="5" t="s">
-        <v>223</v>
+      <c r="A363" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B363" s="7" t="s">
         <v>269</v>
@@ -16629,8 +16766,9 @@
       </c>
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A364" s="5" t="s">
-        <v>223</v>
+      <c r="A364" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B364" s="7" t="s">
         <v>272</v>
@@ -16667,8 +16805,9 @@
       </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A365" s="5" t="s">
-        <v>223</v>
+      <c r="A365" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B365" s="7" t="s">
         <v>280</v>
@@ -16705,8 +16844,9 @@
       </c>
     </row>
     <row r="366" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A366" s="5" t="s">
-        <v>223</v>
+      <c r="A366" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B366" s="7" t="s">
         <v>282</v>
@@ -16743,8 +16883,9 @@
       </c>
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A367" s="5" t="s">
-        <v>223</v>
+      <c r="A367" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B367" s="7" t="s">
         <v>278</v>
@@ -16781,8 +16922,9 @@
       </c>
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A368" s="5" t="s">
-        <v>223</v>
+      <c r="A368" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B368" s="7" t="s">
         <v>277</v>
@@ -16817,8 +16959,9 @@
       </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A369" s="5" t="s">
-        <v>223</v>
+      <c r="A369" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B369" s="7" t="s">
         <v>273</v>
@@ -16853,8 +16996,9 @@
       </c>
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A370" s="5" t="s">
-        <v>223</v>
+      <c r="A370" s="5" t="str">
+        <f>IFERROR(Students!B44, "Student Not Found")</f>
+        <v>Carlo Mendoza</v>
       </c>
       <c r="B370" s="7" t="s">
         <v>275</v>
@@ -16928,8 +17072,9 @@
       </c>
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A372" s="5" t="s">
-        <v>233</v>
+      <c r="A372" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B372" s="7" t="s">
         <v>269</v>
@@ -16966,8 +17111,9 @@
       </c>
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A373" s="5" t="s">
-        <v>233</v>
+      <c r="A373" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B373" s="7" t="s">
         <v>272</v>
@@ -17004,8 +17150,9 @@
       </c>
     </row>
     <row r="374" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A374" s="5" t="s">
-        <v>233</v>
+      <c r="A374" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B374" s="7" t="s">
         <v>280</v>
@@ -17042,8 +17189,9 @@
       </c>
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A375" s="5" t="s">
-        <v>233</v>
+      <c r="A375" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B375" s="7" t="s">
         <v>282</v>
@@ -17080,8 +17228,9 @@
       </c>
     </row>
     <row r="376" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A376" s="5" t="s">
-        <v>233</v>
+      <c r="A376" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B376" s="7" t="s">
         <v>278</v>
@@ -17118,8 +17267,9 @@
       </c>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A377" s="5" t="s">
-        <v>233</v>
+      <c r="A377" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B377" s="7" t="s">
         <v>277</v>
@@ -17154,8 +17304,9 @@
       </c>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A378" s="5" t="s">
-        <v>233</v>
+      <c r="A378" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B378" s="7" t="s">
         <v>273</v>
@@ -17190,8 +17341,9 @@
       </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A379" s="5" t="s">
-        <v>233</v>
+      <c r="A379" s="5" t="str">
+        <f>IFERROR(Students!B46, "Student Not Found")</f>
+        <v>Carlo Morales</v>
       </c>
       <c r="B379" s="7" t="s">
         <v>275</v>
@@ -17265,8 +17417,9 @@
       </c>
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A381" s="5" t="s">
-        <v>248</v>
+      <c r="A381" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B381" s="7" t="s">
         <v>269</v>
@@ -17303,8 +17456,9 @@
       </c>
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A382" s="5" t="s">
-        <v>248</v>
+      <c r="A382" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B382" s="7" t="s">
         <v>272</v>
@@ -17341,8 +17495,9 @@
       </c>
     </row>
     <row r="383" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A383" s="5" t="s">
-        <v>248</v>
+      <c r="A383" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B383" s="7" t="s">
         <v>280</v>
@@ -17379,8 +17534,9 @@
       </c>
     </row>
     <row r="384" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A384" s="5" t="s">
-        <v>248</v>
+      <c r="A384" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B384" s="7" t="s">
         <v>282</v>
@@ -17417,8 +17573,9 @@
       </c>
     </row>
     <row r="385" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A385" s="5" t="s">
-        <v>248</v>
+      <c r="A385" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B385" s="7" t="s">
         <v>278</v>
@@ -17455,8 +17612,9 @@
       </c>
     </row>
     <row r="386" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A386" s="5" t="s">
-        <v>248</v>
+      <c r="A386" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B386" s="7" t="s">
         <v>277</v>
@@ -17491,8 +17649,9 @@
       </c>
     </row>
     <row r="387" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A387" s="5" t="s">
-        <v>248</v>
+      <c r="A387" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B387" s="7" t="s">
         <v>273</v>
@@ -17527,8 +17686,9 @@
       </c>
     </row>
     <row r="388" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A388" s="5" t="s">
-        <v>248</v>
+      <c r="A388" s="5" t="str">
+        <f>IFERROR(Students!B49, "Student Not Found")</f>
+        <v>Carlo Perez</v>
       </c>
       <c r="B388" s="7" t="s">
         <v>275</v>
@@ -17602,8 +17762,9 @@
       </c>
     </row>
     <row r="390" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A390" s="5" t="s">
-        <v>203</v>
+      <c r="A390" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B390" s="7" t="s">
         <v>269</v>
@@ -17640,8 +17801,9 @@
       </c>
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A391" s="5" t="s">
-        <v>203</v>
+      <c r="A391" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B391" s="7" t="s">
         <v>272</v>
@@ -17678,8 +17840,9 @@
       </c>
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A392" s="5" t="s">
-        <v>203</v>
+      <c r="A392" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B392" s="7" t="s">
         <v>280</v>
@@ -17716,8 +17879,9 @@
       </c>
     </row>
     <row r="393" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A393" s="5" t="s">
-        <v>203</v>
+      <c r="A393" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B393" s="7" t="s">
         <v>282</v>
@@ -17754,8 +17918,9 @@
       </c>
     </row>
     <row r="394" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A394" s="5" t="s">
-        <v>203</v>
+      <c r="A394" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B394" s="7" t="s">
         <v>278</v>
@@ -17792,8 +17957,9 @@
       </c>
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A395" s="5" t="s">
-        <v>203</v>
+      <c r="A395" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B395" s="7" t="s">
         <v>277</v>
@@ -17828,8 +17994,9 @@
       </c>
     </row>
     <row r="396" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A396" s="5" t="s">
-        <v>203</v>
+      <c r="A396" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B396" s="7" t="s">
         <v>273</v>
@@ -17864,8 +18031,9 @@
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A397" s="5" t="s">
-        <v>203</v>
+      <c r="A397" s="5" t="str">
+        <f>IFERROR(Students!B40, "Student Not Found")</f>
+        <v>Carlo Ramos</v>
       </c>
       <c r="B397" s="7" t="s">
         <v>275</v>
@@ -17939,8 +18107,9 @@
       </c>
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A399" s="5" t="s">
-        <v>183</v>
+      <c r="A399" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B399" s="7" t="s">
         <v>269</v>
@@ -17977,8 +18146,9 @@
       </c>
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A400" s="5" t="s">
-        <v>183</v>
+      <c r="A400" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B400" s="7" t="s">
         <v>272</v>
@@ -18015,8 +18185,9 @@
       </c>
     </row>
     <row r="401" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A401" s="5" t="s">
-        <v>183</v>
+      <c r="A401" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B401" s="7" t="s">
         <v>280</v>
@@ -18053,8 +18224,9 @@
       </c>
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A402" s="5" t="s">
-        <v>183</v>
+      <c r="A402" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B402" s="8" t="s">
         <v>282</v>
@@ -18091,8 +18263,9 @@
       </c>
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A403" s="5" t="s">
-        <v>183</v>
+      <c r="A403" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B403" s="8" t="s">
         <v>278</v>
@@ -18129,8 +18302,9 @@
       </c>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A404" s="5" t="s">
-        <v>183</v>
+      <c r="A404" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B404" s="8" t="s">
         <v>277</v>
@@ -18167,8 +18341,9 @@
       </c>
     </row>
     <row r="405" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A405" s="5" t="s">
-        <v>183</v>
+      <c r="A405" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B405" s="8" t="s">
         <v>273</v>
@@ -18203,8 +18378,9 @@
       </c>
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A406" s="5" t="s">
-        <v>183</v>
+      <c r="A406" s="5" t="str">
+        <f>IFERROR(Students!B36, "Student Not Found")</f>
+        <v>Carlo Reyes</v>
       </c>
       <c r="B406" s="8" t="s">
         <v>275</v>
@@ -18278,8 +18454,9 @@
       </c>
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A408" s="5" t="s">
-        <v>218</v>
+      <c r="A408" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B408" s="8" t="s">
         <v>269</v>
@@ -18316,8 +18493,9 @@
       </c>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A409" s="5" t="s">
-        <v>218</v>
+      <c r="A409" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B409" s="8" t="s">
         <v>272</v>
@@ -18354,8 +18532,9 @@
       </c>
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A410" s="5" t="s">
-        <v>218</v>
+      <c r="A410" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B410" s="8" t="s">
         <v>280</v>
@@ -18392,8 +18571,9 @@
       </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A411" s="5" t="s">
-        <v>218</v>
+      <c r="A411" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B411" s="8" t="s">
         <v>282</v>
@@ -18430,8 +18610,9 @@
       </c>
     </row>
     <row r="412" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A412" s="5" t="s">
-        <v>218</v>
+      <c r="A412" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B412" s="8" t="s">
         <v>278</v>
@@ -18468,8 +18649,9 @@
       </c>
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A413" s="5" t="s">
-        <v>218</v>
+      <c r="A413" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B413" s="8" t="s">
         <v>277</v>
@@ -18504,8 +18686,9 @@
       </c>
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A414" s="5" t="s">
-        <v>218</v>
+      <c r="A414" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B414" s="8" t="s">
         <v>273</v>
@@ -18540,8 +18723,9 @@
       </c>
     </row>
     <row r="415" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A415" s="5" t="s">
-        <v>218</v>
+      <c r="A415" s="5" t="str">
+        <f>IFERROR(Students!B43, "Student Not Found")</f>
+        <v>Carlo Rivera</v>
       </c>
       <c r="B415" s="8" t="s">
         <v>275</v>
@@ -18577,7 +18761,7 @@
     </row>
     <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A416" s="5" t="str">
-        <f>IFERROR(Students!B34, "Student Not Found")</f>
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
         <v>Carlo Santos</v>
       </c>
       <c r="B416" s="8" t="s">
@@ -18615,8 +18799,9 @@
       </c>
     </row>
     <row r="417" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A417" s="5" t="s">
-        <v>173</v>
+      <c r="A417" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B417" s="8" t="s">
         <v>269</v>
@@ -18653,8 +18838,9 @@
       </c>
     </row>
     <row r="418" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A418" s="5" t="s">
-        <v>173</v>
+      <c r="A418" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B418" s="8" t="s">
         <v>272</v>
@@ -18691,8 +18877,9 @@
       </c>
     </row>
     <row r="419" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A419" s="5" t="s">
-        <v>173</v>
+      <c r="A419" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B419" s="8" t="s">
         <v>280</v>
@@ -18729,8 +18916,9 @@
       </c>
     </row>
     <row r="420" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A420" s="5" t="s">
-        <v>173</v>
+      <c r="A420" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B420" s="8" t="s">
         <v>282</v>
@@ -18767,8 +18955,9 @@
       </c>
     </row>
     <row r="421" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A421" s="5" t="s">
-        <v>173</v>
+      <c r="A421" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B421" s="8" t="s">
         <v>278</v>
@@ -18805,8 +18994,9 @@
       </c>
     </row>
     <row r="422" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A422" s="5" t="s">
-        <v>173</v>
+      <c r="A422" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B422" s="8" t="s">
         <v>277</v>
@@ -18843,8 +19033,9 @@
       </c>
     </row>
     <row r="423" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A423" s="5" t="s">
-        <v>173</v>
+      <c r="A423" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B423" s="8" t="s">
         <v>273</v>
@@ -18879,8 +19070,9 @@
       </c>
     </row>
     <row r="424" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A424" s="5" t="s">
-        <v>173</v>
+      <c r="A424" s="5" t="str">
+        <f>IFERROR(Students!B$34, "Student Not Found")</f>
+        <v>Carlo Santos</v>
       </c>
       <c r="B424" s="8" t="s">
         <v>275</v>
@@ -18916,7 +19108,7 @@
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A425" s="5" t="str">
-        <f>IFERROR(Students!B42, "Student Not Found")</f>
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
         <v>Carlo Torres</v>
       </c>
       <c r="B425" s="8" t="s">
@@ -18954,8 +19146,9 @@
       </c>
     </row>
     <row r="426" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A426" s="5" t="s">
-        <v>213</v>
+      <c r="A426" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B426" s="8" t="s">
         <v>269</v>
@@ -18992,8 +19185,9 @@
       </c>
     </row>
     <row r="427" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A427" s="5" t="s">
-        <v>213</v>
+      <c r="A427" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B427" s="8" t="s">
         <v>272</v>
@@ -19030,8 +19224,9 @@
       </c>
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A428" s="5" t="s">
-        <v>213</v>
+      <c r="A428" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B428" s="8" t="s">
         <v>280</v>
@@ -19068,8 +19263,9 @@
       </c>
     </row>
     <row r="429" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A429" s="5" t="s">
-        <v>213</v>
+      <c r="A429" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B429" s="8" t="s">
         <v>282</v>
@@ -19106,8 +19302,9 @@
       </c>
     </row>
     <row r="430" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A430" s="5" t="s">
-        <v>213</v>
+      <c r="A430" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B430" s="8" t="s">
         <v>278</v>
@@ -19144,8 +19341,9 @@
       </c>
     </row>
     <row r="431" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A431" s="5" t="s">
-        <v>213</v>
+      <c r="A431" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B431" s="8" t="s">
         <v>277</v>
@@ -19180,8 +19378,9 @@
       </c>
     </row>
     <row r="432" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A432" s="5" t="s">
-        <v>213</v>
+      <c r="A432" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B432" s="8" t="s">
         <v>273</v>
@@ -19216,8 +19415,9 @@
       </c>
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A433" s="5" t="s">
-        <v>213</v>
+      <c r="A433" s="5" t="str">
+        <f>IFERROR(Students!B$42, "Student Not Found")</f>
+        <v>Carlo Torres</v>
       </c>
       <c r="B433" s="8" t="s">
         <v>275</v>
@@ -19253,7 +19453,7 @@
     </row>
     <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" s="5" t="str">
-        <f>IFERROR(Students!B51, "Student Not Found")</f>
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
         <v>Dina Garcia</v>
       </c>
       <c r="B434" s="8" t="s">
@@ -19291,8 +19491,9 @@
       </c>
     </row>
     <row r="435" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A435" s="5" t="s">
-        <v>258</v>
+      <c r="A435" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B435" s="8" t="s">
         <v>269</v>
@@ -19329,8 +19530,9 @@
       </c>
     </row>
     <row r="436" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A436" s="5" t="s">
-        <v>258</v>
+      <c r="A436" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B436" s="8" t="s">
         <v>272</v>
@@ -19367,8 +19569,9 @@
       </c>
     </row>
     <row r="437" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A437" s="5" t="s">
-        <v>258</v>
+      <c r="A437" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B437" s="8" t="s">
         <v>280</v>
@@ -19405,8 +19608,9 @@
       </c>
     </row>
     <row r="438" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A438" s="5" t="s">
-        <v>258</v>
+      <c r="A438" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B438" s="8" t="s">
         <v>282</v>
@@ -19443,8 +19647,9 @@
       </c>
     </row>
     <row r="439" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A439" s="5" t="s">
-        <v>258</v>
+      <c r="A439" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B439" s="8" t="s">
         <v>278</v>
@@ -19481,8 +19686,9 @@
       </c>
     </row>
     <row r="440" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A440" s="5" t="s">
-        <v>258</v>
+      <c r="A440" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B440" s="8" t="s">
         <v>277</v>
@@ -19517,8 +19723,9 @@
       </c>
     </row>
     <row r="441" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A441" s="5" t="s">
-        <v>258</v>
+      <c r="A441" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B441" s="8" t="s">
         <v>273</v>
@@ -19553,8 +19760,9 @@
       </c>
     </row>
     <row r="442" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A442" s="5" t="s">
-        <v>258</v>
+      <c r="A442" s="5" t="str">
+        <f>IFERROR(Students!B$51, "Student Not Found")</f>
+        <v>Dina Garcia</v>
       </c>
       <c r="B442" s="8" t="s">
         <v>275</v>
@@ -19590,7 +19798,7 @@
     </row>
     <row r="443" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A443" s="5" t="str">
-        <f>IFERROR(Students!B50, "Student Not Found")</f>
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
         <v>Dina Santos</v>
       </c>
       <c r="B443" s="8" t="s">
@@ -19628,8 +19836,9 @@
       </c>
     </row>
     <row r="444" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A444" s="5" t="s">
-        <v>253</v>
+      <c r="A444" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B444" s="8" t="s">
         <v>269</v>
@@ -19666,8 +19875,9 @@
       </c>
     </row>
     <row r="445" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A445" s="5" t="s">
-        <v>253</v>
+      <c r="A445" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B445" s="8" t="s">
         <v>272</v>
@@ -19704,8 +19914,9 @@
       </c>
     </row>
     <row r="446" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A446" s="5" t="s">
-        <v>253</v>
+      <c r="A446" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B446" s="8" t="s">
         <v>280</v>
@@ -19742,8 +19953,9 @@
       </c>
     </row>
     <row r="447" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A447" s="5" t="s">
-        <v>253</v>
+      <c r="A447" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B447" s="8" t="s">
         <v>282</v>
@@ -19780,8 +19992,9 @@
       </c>
     </row>
     <row r="448" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A448" s="5" t="s">
-        <v>253</v>
+      <c r="A448" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B448" s="8" t="s">
         <v>278</v>
@@ -19818,8 +20031,9 @@
       </c>
     </row>
     <row r="449" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A449" s="5" t="s">
-        <v>253</v>
+      <c r="A449" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B449" s="8" t="s">
         <v>277</v>
@@ -19854,8 +20068,9 @@
       </c>
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A450" s="5" t="s">
-        <v>253</v>
+      <c r="A450" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B450" s="8" t="s">
         <v>273</v>
@@ -19890,8 +20105,9 @@
       </c>
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A451" s="5" t="s">
-        <v>253</v>
+      <c r="A451" s="5" t="str">
+        <f>IFERROR(Students!B$50, "Student Not Found")</f>
+        <v>Dina Santos</v>
       </c>
       <c r="B451" s="8" t="s">
         <v>275</v>
@@ -19925,6 +20141,330 @@
         <v>274</v>
       </c>
     </row>
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A452" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B452" t="s">
+        <v>281</v>
+      </c>
+      <c r="C452">
+        <v>96</v>
+      </c>
+      <c r="D452">
+        <v>98</v>
+      </c>
+      <c r="E452">
+        <v>84</v>
+      </c>
+      <c r="F452">
+        <v>80</v>
+      </c>
+      <c r="G452" s="9">
+        <v>89.5</v>
+      </c>
+      <c r="H452" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="I452" t="s">
+        <v>285</v>
+      </c>
+      <c r="J452" t="s">
+        <v>270</v>
+      </c>
+      <c r="K452" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A453" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B453" t="s">
+        <v>269</v>
+      </c>
+      <c r="C453">
+        <v>87</v>
+      </c>
+      <c r="D453">
+        <v>99</v>
+      </c>
+      <c r="E453">
+        <v>80</v>
+      </c>
+      <c r="F453">
+        <v>92</v>
+      </c>
+      <c r="G453" s="9">
+        <v>89.5</v>
+      </c>
+      <c r="H453" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="I453" t="s">
+        <v>285</v>
+      </c>
+      <c r="J453" t="s">
+        <v>276</v>
+      </c>
+      <c r="K453" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A454" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B454" t="s">
+        <v>272</v>
+      </c>
+      <c r="C454">
+        <v>85</v>
+      </c>
+      <c r="D454">
+        <v>95</v>
+      </c>
+      <c r="E454">
+        <v>75</v>
+      </c>
+      <c r="F454">
+        <v>97</v>
+      </c>
+      <c r="G454" s="9">
+        <v>88</v>
+      </c>
+      <c r="H454" s="9">
+        <v>2</v>
+      </c>
+      <c r="I454" t="s">
+        <v>285</v>
+      </c>
+      <c r="J454" t="s">
+        <v>270</v>
+      </c>
+      <c r="K454" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A455" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B455" t="s">
+        <v>280</v>
+      </c>
+      <c r="C455">
+        <v>76</v>
+      </c>
+      <c r="D455">
+        <v>75</v>
+      </c>
+      <c r="E455">
+        <v>78</v>
+      </c>
+      <c r="F455">
+        <v>80</v>
+      </c>
+      <c r="G455" s="9">
+        <v>77.25</v>
+      </c>
+      <c r="H455" s="9">
+        <v>2.75</v>
+      </c>
+      <c r="I455" t="s">
+        <v>285</v>
+      </c>
+      <c r="J455" t="s">
+        <v>270</v>
+      </c>
+      <c r="K455" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A456" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B456" t="s">
+        <v>282</v>
+      </c>
+      <c r="C456">
+        <v>89</v>
+      </c>
+      <c r="D456">
+        <v>76</v>
+      </c>
+      <c r="E456">
+        <v>79</v>
+      </c>
+      <c r="F456">
+        <v>94</v>
+      </c>
+      <c r="G456" s="9">
+        <v>84.5</v>
+      </c>
+      <c r="H456" s="9">
+        <v>2.25</v>
+      </c>
+      <c r="I456" t="s">
+        <v>285</v>
+      </c>
+      <c r="J456" t="s">
+        <v>279</v>
+      </c>
+      <c r="K456" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A457" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B457" t="s">
+        <v>278</v>
+      </c>
+      <c r="C457">
+        <v>98</v>
+      </c>
+      <c r="D457">
+        <v>80</v>
+      </c>
+      <c r="E457">
+        <v>89</v>
+      </c>
+      <c r="F457">
+        <v>79</v>
+      </c>
+      <c r="G457" s="9">
+        <v>86.5</v>
+      </c>
+      <c r="H457" s="9">
+        <v>2</v>
+      </c>
+      <c r="I457" t="s">
+        <v>285</v>
+      </c>
+      <c r="J457" t="s">
+        <v>270</v>
+      </c>
+      <c r="K457" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A458" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B458" t="s">
+        <v>277</v>
+      </c>
+      <c r="C458">
+        <v>77</v>
+      </c>
+      <c r="D458">
+        <v>92</v>
+      </c>
+      <c r="E458">
+        <v>84</v>
+      </c>
+      <c r="F458">
+        <v>91</v>
+      </c>
+      <c r="G458" s="9">
+        <v>86</v>
+      </c>
+      <c r="H458" s="9">
+        <v>2</v>
+      </c>
+      <c r="I458" t="s">
+        <v>285</v>
+      </c>
+      <c r="J458" t="s">
+        <v>276</v>
+      </c>
+      <c r="K458" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A459" s="5" t="str">
+        <f>IFERROR(Students!B52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B459" t="s">
+        <v>273</v>
+      </c>
+      <c r="C459">
+        <v>77</v>
+      </c>
+      <c r="D459">
+        <v>92</v>
+      </c>
+      <c r="E459">
+        <v>84</v>
+      </c>
+      <c r="F459">
+        <v>91</v>
+      </c>
+      <c r="G459" s="9">
+        <v>86</v>
+      </c>
+      <c r="H459" s="9">
+        <v>2</v>
+      </c>
+      <c r="I459" t="s">
+        <v>285</v>
+      </c>
+      <c r="J459" t="s">
+        <v>276</v>
+      </c>
+      <c r="K459" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A460" s="5" t="str">
+        <f>IFERROR(Students!B$52, "Student Not Found")</f>
+        <v>Adrian Angeles</v>
+      </c>
+      <c r="B460" t="s">
+        <v>275</v>
+      </c>
+      <c r="C460">
+        <v>79</v>
+      </c>
+      <c r="D460">
+        <v>96</v>
+      </c>
+      <c r="E460">
+        <v>92</v>
+      </c>
+      <c r="F460">
+        <v>90</v>
+      </c>
+      <c r="G460" s="9">
+        <v>89.25</v>
+      </c>
+      <c r="H460" s="9">
+        <v>1.75</v>
+      </c>
+      <c r="I460" t="s">
+        <v>285</v>
+      </c>
+      <c r="J460" t="s">
+        <v>270</v>
+      </c>
+      <c r="K460" t="s">
+        <v>274</v>
+      </c>
+    </row>
     <row r="602" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O602" s="3"/>
     </row>
@@ -20905,30 +21445,30 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="I2:I451">
-    <cfRule type="expression" dxfId="3" priority="5">
+  <conditionalFormatting sqref="I2:I460">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>I2="PASSED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>I2="Failed"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
       <formula>$I$2="PASSED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="8" stopIfTrue="1">
       <formula>$I$2="FAILED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K340">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$I$2="PASSED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M602:N927">
-    <cfRule type="expression" dxfId="5" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="9" stopIfTrue="1">
       <formula>$I$2="PASSED"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$I$2="FAILED"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>